<commit_message>
update import excel, course schema; chg xls format
</commit_message>
<xml_diff>
--- a/server/uploads/import.xlsx
+++ b/server/uploads/import.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+  <si>
+    <t>Sem</t>
+  </si>
   <si>
     <t>CourseCode</t>
   </si>
   <si>
-    <t>courseName</t>
+    <t>CourseName</t>
   </si>
   <si>
     <t>Type</t>
@@ -49,7 +52,7 @@
     <t>ABCD1234</t>
   </si>
   <si>
-    <t>Intro to Machine Learning X</t>
+    <t>intro to fucking</t>
   </si>
   <si>
     <t>L</t>
@@ -70,22 +73,22 @@
     <t>This is fucking good class</t>
   </si>
   <si>
+    <t>EFGH5673</t>
+  </si>
+  <si>
+    <t>intro to puss</t>
+  </si>
+  <si>
+    <t>ALAN</t>
+  </si>
+  <si>
+    <t>THU-12:00-13:30,       WED-11:00-12:30,FRI-10:50-11:50</t>
+  </si>
+  <si>
     <t>EFGH5678</t>
   </si>
   <si>
-    <t>Advanced Introduction to Introduction</t>
-  </si>
-  <si>
-    <t>ALAN</t>
-  </si>
-  <si>
-    <t>THU-12:00-13:30,       WED-11:00-12:30,FRI-10:50-11:50</t>
-  </si>
-  <si>
-    <t>JKEL5679</t>
-  </si>
-  <si>
-    <t>Very Unreal Analysis</t>
+    <t>intro to dick</t>
   </si>
   <si>
     <t xml:space="preserve">THU-12:00-13:30,WED-11:00-12:30,FRI-10:50-11:50                </t>
@@ -138,13 +141,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -454,25 +460,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,19 +489,19 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -503,10 +510,13 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -514,20 +524,20 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2">
-        <v>1100</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>100</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -535,69 +545,78 @@
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3">
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2">
         <v>50</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="3">
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2">
         <v>50</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rm date from course schema&update related code
</commit_message>
<xml_diff>
--- a/server/uploads/import.xlsx
+++ b/server/uploads/import.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>CourseCode</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Instructor</t>
   </si>
   <si>
-    <t>Dates</t>
-  </si>
-  <si>
     <t>Seat</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t>KKL</t>
-  </si>
-  <si>
-    <t>2023-02-01,2023-02-02,2023-02-03,2023-02-08</t>
   </si>
   <si>
     <t>4-00-02,3-03-04</t>
@@ -457,7 +451,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -467,11 +461,10 @@
     <col min="2" max="2" style="3" width="17.719285714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -487,10 +480,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -498,96 +491,84 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2">
-        <v>100</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="2">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2">
-        <v>50</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2">
-        <v>50</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>